<commit_message>
new design based on type of configuration
</commit_message>
<xml_diff>
--- a/Documentation/LimeAPI_descruption.xlsx
+++ b/Documentation/LimeAPI_descruption.xlsx
@@ -907,6 +907,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1003,9 +1004,9 @@
   <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="K73" activeCellId="0" sqref="K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1014,7 +1015,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="48.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.6"/>
@@ -1022,8 +1023,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="11.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="17.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="17.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="11.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="9.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="43.25"/>

</xml_diff>